<commit_message>
working version of 2 layer model
</commit_message>
<xml_diff>
--- a/network models.xlsx
+++ b/network models.xlsx
@@ -476,7 +476,7 @@
   <dimension ref="B2:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -642,7 +642,7 @@
     <row r="18" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>